<commit_message>
Added lifetime consideration in Future_2015_industry file
</commit_message>
<xml_diff>
--- a/Data/3_LT_RECC_ProductLifetime_industry_V1.0.xlsx
+++ b/Data/3_LT_RECC_ProductLifetime_industry_V1.0.xlsx
@@ -760,7 +760,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
@@ -772,7 +772,7 @@
     <col bestFit="1" customWidth="1" max="2" min="2" style="15" width="70.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -783,7 +783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -797,7 +797,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -811,7 +811,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:8">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -825,7 +825,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -839,7 +839,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:8">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
@@ -853,7 +853,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:8">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
@@ -867,7 +867,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:8">
       <c r="A8" s="8" t="s">
         <v>20</v>
       </c>
@@ -881,7 +881,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:8">
       <c r="A9" s="8" t="s">
         <v>23</v>
       </c>
@@ -895,7 +895,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:8">
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
@@ -909,7 +909,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:8">
       <c r="A11" s="8" t="s">
         <v>28</v>
       </c>
@@ -923,7 +923,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:8">
       <c r="A12" s="5" t="s">
         <v>30</v>
       </c>
@@ -937,7 +937,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:8">
       <c r="A13" s="5" t="s">
         <v>32</v>
       </c>
@@ -951,7 +951,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:8">
       <c r="A14" s="5" t="s">
         <v>35</v>
       </c>
@@ -965,7 +965,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:8">
       <c r="A15" s="5" t="s">
         <v>37</v>
       </c>
@@ -979,37 +979,37 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:8">
       <c r="A16" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E16" s="14" t="n"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:8">
       <c r="A17" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E17" s="14" t="n"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:8">
       <c r="A18" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E18" s="14" t="n"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:8">
       <c r="A19" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E19" s="14" t="n"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:8">
       <c r="A20" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E20" s="14" t="n"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:8">
       <c r="A21" s="5" t="s">
         <v>41</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:8">
       <c r="A22" s="5" t="s">
         <v>44</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:8">
       <c r="A23" s="16" t="s">
         <v>48</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:8">
       <c r="A24" s="16" t="s">
         <v>21</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:8">
       <c r="A25" s="18" t="s">
         <v>56</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:8">
       <c r="C26" s="16" t="s">
         <v>61</v>
       </c>
@@ -1118,22 +1118,22 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:8">
       <c r="E27" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:8">
       <c r="E28" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:8">
       <c r="E29" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:8">
       <c r="E30" s="14" t="s">
         <v>1</v>
       </c>

</xml_diff>